<commit_message>
extracts and cleans data -> removes html tags, groups by 30minute intervals, joins into a single column, removes most duplicates
</commit_message>
<xml_diff>
--- a/filtered_traffic_2022_01_30_cleaned.xlsx
+++ b/filtered_traffic_2022_01_30_cleaned.xlsx
@@ -589,7 +589,7 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -638,7 +638,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -687,7 +687,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -736,7 +736,7 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -785,7 +785,7 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -834,7 +834,7 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
@@ -887,7 +887,7 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
@@ -940,7 +940,7 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
@@ -993,7 +993,7 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
@@ -1046,7 +1046,7 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -1099,7 +1099,7 @@
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
@@ -1152,7 +1152,7 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F13" t="inlineStr"/>
@@ -1205,7 +1205,7 @@
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F14" t="inlineStr"/>
@@ -1258,7 +1258,7 @@
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F15" t="inlineStr"/>
@@ -1311,7 +1311,7 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F16" t="inlineStr"/>
@@ -1364,7 +1364,7 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F17" t="inlineStr"/>
@@ -1417,7 +1417,7 @@
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F18" t="inlineStr"/>
@@ -1470,7 +1470,7 @@
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F19" t="inlineStr"/>
@@ -1523,7 +1523,7 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F20" t="inlineStr"/>
@@ -1576,7 +1576,7 @@
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na dolenjski avtocesti pred priključkom Smednik v smeri Obrežja, predmet na vozišču, oviran promet. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F21" t="inlineStr"/>
@@ -1629,7 +1629,7 @@
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F22" t="inlineStr"/>
@@ -1678,7 +1678,7 @@
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F23" t="inlineStr"/>
@@ -1727,7 +1727,7 @@
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F24" t="inlineStr"/>
@@ -1776,7 +1776,7 @@
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F25" t="inlineStr"/>
@@ -1825,7 +1825,7 @@
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F26" t="inlineStr"/>
@@ -1874,7 +1874,7 @@
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F27" t="inlineStr"/>
@@ -1923,7 +1923,7 @@
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F28" t="inlineStr"/>
@@ -1972,7 +1972,7 @@
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F29" t="inlineStr"/>
@@ -2021,7 +2021,7 @@
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F30" t="inlineStr"/>
@@ -2070,7 +2070,7 @@
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F31" t="inlineStr"/>
@@ -2119,7 +2119,7 @@
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F32" t="inlineStr"/>
@@ -2168,7 +2168,7 @@
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F33" t="inlineStr"/>
@@ -2217,7 +2217,7 @@
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F34" t="inlineStr"/>
@@ -2266,7 +2266,7 @@
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F35" t="inlineStr"/>
@@ -2315,7 +2315,7 @@
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F36" t="inlineStr"/>
@@ -2364,7 +2364,7 @@
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F37" t="inlineStr"/>
@@ -2413,7 +2413,7 @@
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F38" t="inlineStr"/>
@@ -2462,7 +2462,7 @@
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F39" t="inlineStr"/>
@@ -2511,7 +2511,7 @@
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F40" t="inlineStr"/>
@@ -2560,7 +2560,7 @@
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F41" t="inlineStr"/>
@@ -2609,7 +2609,7 @@
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F42" t="inlineStr"/>
@@ -2658,7 +2658,7 @@
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F43" t="inlineStr"/>
@@ -2707,7 +2707,7 @@
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F44" t="inlineStr"/>
@@ -2756,7 +2756,7 @@
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F45" t="inlineStr"/>
@@ -2805,7 +2805,7 @@
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F46" t="inlineStr"/>
@@ -2854,7 +2854,7 @@
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F47" t="inlineStr"/>
@@ -2903,7 +2903,7 @@
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F48" t="inlineStr"/>
@@ -2952,7 +2952,7 @@
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F49" t="inlineStr"/>
@@ -3001,7 +3001,7 @@
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F50" t="inlineStr"/>
@@ -3050,7 +3050,7 @@
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F51" t="inlineStr"/>
@@ -3099,7 +3099,7 @@
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F52" t="inlineStr"/>
@@ -3148,7 +3148,7 @@
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F53" t="inlineStr"/>
@@ -3197,7 +3197,7 @@
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F54" t="inlineStr"/>
@@ -3246,7 +3246,7 @@
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F55" t="inlineStr"/>
@@ -3295,7 +3295,7 @@
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F56" t="inlineStr"/>
@@ -3344,7 +3344,7 @@
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F57" t="inlineStr"/>
@@ -3393,7 +3393,7 @@
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F58" t="inlineStr"/>
@@ -3442,7 +3442,7 @@
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F59" t="inlineStr"/>
@@ -3491,7 +3491,7 @@
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F60" t="inlineStr"/>
@@ -3540,7 +3540,7 @@
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F61" t="inlineStr"/>
@@ -3589,7 +3589,7 @@
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
@@ -3638,7 +3638,7 @@
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F63" t="inlineStr"/>
@@ -3687,7 +3687,7 @@
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F64" t="inlineStr"/>
@@ -3736,7 +3736,7 @@
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F65" t="inlineStr"/>
@@ -3785,7 +3785,7 @@
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F66" t="inlineStr"/>
@@ -3834,7 +3834,7 @@
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F67" t="inlineStr"/>
@@ -3883,7 +3883,7 @@
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F68" t="inlineStr"/>
@@ -3932,7 +3932,7 @@
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F69" t="inlineStr"/>
@@ -3981,7 +3981,7 @@
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F70" t="inlineStr"/>
@@ -4030,7 +4030,7 @@
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F71" t="inlineStr"/>
@@ -4079,7 +4079,7 @@
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes med 8. in 22. uro velja prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Opozorila Danes med 8. in 22. uro velja prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F72" t="inlineStr"/>
@@ -4132,7 +4132,7 @@
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes med 8. in 22. uro velja prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Opozorila Danes med 8. in 22. uro velja prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F73" t="inlineStr"/>
@@ -4185,7 +4185,7 @@
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes med 8. in 22. uro velja prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Opozorila Danes med 8. in 22. uro velja prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F74" t="inlineStr"/>
@@ -4238,7 +4238,7 @@
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na gorenjski avtocesti vozite previdno med obema priključkom za Kranj. Vozniki so opazili žival na cestišču. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes med 8. in 22. uro velja prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na gorenjski avtocesti vozite previdno med obema priključkom za Kranj. Vozniki so opazili žival na cestišču. Opozorila Danes med 8. in 22. uro velja prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F75" t="inlineStr"/>
@@ -4295,7 +4295,7 @@
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na gorenjski avtocesti vozite previdno med obema priključkom za Kranj. Vozniki so opazili žival na cestišču. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na gorenjski avtocesti vozite previdno med obema priključkom za Kranj. Vozniki so opazili žival na cestišču. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F76" t="inlineStr"/>
@@ -4352,7 +4352,7 @@
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Po gorenjski avtocesti vozite previdno:&lt;/strong&gt;&lt;br&gt;- Med obema priključkom za Kranj so vozniki opazili žival na cestišču.&lt;br&gt;- pred Lescami proti Ljubljani pa promet ovira okvarjeno vozilo.  &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Po gorenjski avtocesti vozite previdno: - Med obema priključkom za Kranj so vozniki opazili žival na cestišču. - pred Lescami proti Ljubljani pa promet ovira okvarjeno vozilo. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F77" t="inlineStr"/>
@@ -4409,7 +4409,7 @@
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Po gorenjski avtocesti vozite previdno,&lt;/strong&gt; pred Lescami proti Ljubljani promet ovira okvarjeno vozilo.  &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Po gorenjski avtocesti vozite previdno, pred Lescami proti Ljubljani promet ovira okvarjeno vozilo. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F78" t="inlineStr"/>
@@ -4465,12 +4465,12 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Pozor!&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Predor Karavanke je v obe smeri zaprt zaradi kratkotrajne delovne zapore. &lt;/strong&gt;&lt;/p&gt;</t>
+          <t>Pozor! Predor Karavanke je v obe smeri zaprt zaradi kratkotrajne delovne zapore.</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Po gorenjski avtocesti vozite previdno,&lt;/strong&gt; pred Lescami proti Ljubljani promet ovira okvarjeno vozilo.  &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Po gorenjski avtocesti vozite previdno, pred Lescami proti Ljubljani promet ovira okvarjeno vozilo. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F79" t="inlineStr"/>
@@ -4531,7 +4531,7 @@
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Po gorenjski avtocesti vozite previdno,&lt;/strong&gt; pred Lescami proti Ljubljani promet ovira okvarjeno vozilo.  &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Po gorenjski avtocesti vozite previdno, pred Lescami proti Ljubljani promet ovira okvarjeno vozilo. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F80" t="inlineStr"/>
@@ -4588,7 +4588,7 @@
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F81" t="inlineStr"/>
@@ -4641,7 +4641,7 @@
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F82" t="inlineStr"/>
@@ -4694,7 +4694,7 @@
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F83" t="inlineStr"/>
@@ -4747,7 +4747,7 @@
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na štajerski avtocesti je v predoru Jasovnik proti Ljubljani zaprt vozni pas zaradi okvare vozila.  &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na štajerski avtocesti je v predoru Jasovnik proti Ljubljani zaprt vozni pas zaradi okvare vozila. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F84" t="inlineStr"/>
@@ -4804,7 +4804,7 @@
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na štajerski avtocesti je v predoru Jasovnik proti Ljubljani zaprt vozni pas zaradi okvare vozila.  &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Na štajerski avtocesti je v predoru Jasovnik proti Ljubljani zaprt vozni pas zaradi okvare vozila. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F85" t="inlineStr"/>
@@ -4861,7 +4861,7 @@
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F86" t="inlineStr"/>
@@ -4914,7 +4914,7 @@
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Previdno vozite po glavni cesti Kočevje - Ljubljana med Pijavo Gorico in Vrhom nad Želimljami. Po cesti se sprehaja konj. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Previdno vozite po glavni cesti Kočevje - Ljubljana med Pijavo Gorico in Vrhom nad Želimljami. Po cesti se sprehaja konj. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F87" t="inlineStr"/>
@@ -4971,7 +4971,7 @@
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Previdno vozite po glavni cesti Kočevje - Ljubljana med Pijavo Gorico in Vrhom nad Želimljami. Po cesti se sprehajata konja. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Previdno vozite po glavni cesti Kočevje - Ljubljana med Pijavo Gorico in Vrhom nad Želimljami. Po cesti se sprehajata konja. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F88" t="inlineStr"/>
@@ -5028,7 +5028,7 @@
       <c r="D89" t="inlineStr"/>
       <c r="E89" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Previdno vozite po glavni cesti Kočevje - Ljubljana med Turjakom in Rašico. Po cesti se sprehajata konja. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Previdno vozite po glavni cesti Kočevje - Ljubljana med Turjakom in Rašico. Po cesti se sprehajata konja. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F89" t="inlineStr"/>
@@ -5085,7 +5085,7 @@
       <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Previdno vozite po glavni cesti Kočevje - Ljubljana med Turjakom in Rašico. Po cesti se sprehajata konja. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Previdno vozite po glavni cesti Kočevje - Ljubljana med Turjakom in Rašico. Po cesti se sprehajata konja. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F90" t="inlineStr"/>
@@ -5142,7 +5142,7 @@
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Ovire&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Previdno vozite po glavni cesti Kočevje - Ljubljana med Turjakom in Rašico. Po cesti se sprehajata konja. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Zastoji&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na cesti  Bled - Lesce na Bledu. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Ovire Previdno vozite po glavni cesti Kočevje - Ljubljana med Turjakom in Rašico. Po cesti se sprehajata konja. Zastoji Na cesti Bled - Lesce na Bledu. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F91" t="inlineStr"/>
@@ -5156,7 +5156,7 @@
       <c r="N91" t="inlineStr"/>
       <c r="O91" t="inlineStr">
         <is>
-          <t>Na cesti  Bled - Lesce na Bledu.</t>
+          <t>Na cesti Bled - Lesce na Bledu.</t>
         </is>
       </c>
       <c r="P91" t="inlineStr"/>
@@ -5203,7 +5203,7 @@
       <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Zastoji&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na cesti  Bled - Lesce na Bledu. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Zastoji Na cesti Bled - Lesce na Bledu. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F92" t="inlineStr"/>
@@ -5217,7 +5217,7 @@
       <c r="N92" t="inlineStr"/>
       <c r="O92" t="inlineStr">
         <is>
-          <t>Na cesti  Bled - Lesce na Bledu.</t>
+          <t>Na cesti Bled - Lesce na Bledu.</t>
         </is>
       </c>
       <c r="P92" t="inlineStr"/>
@@ -5260,7 +5260,7 @@
       <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Nesreče&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta slovenske Konjice - Tepanje je zaprta Dobrnežu. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Zastoji&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na cesti  Bled - Lesce na Bledu. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Nesreče Regionalna cesta slovenske Konjice - Tepanje je zaprta Dobrnežu. Zastoji Na cesti Bled - Lesce na Bledu. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F93" t="inlineStr"/>
@@ -5278,7 +5278,7 @@
       <c r="N93" t="inlineStr"/>
       <c r="O93" t="inlineStr">
         <is>
-          <t>Na cesti  Bled - Lesce na Bledu.</t>
+          <t>Na cesti Bled - Lesce na Bledu.</t>
         </is>
       </c>
       <c r="P93" t="inlineStr"/>
@@ -5321,7 +5321,7 @@
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Nesreče&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta slovenske Konjice - Tepanje je zaprta Dobrnežu. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Zastoji&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na cesti  Bled - Lesce na Bledu. &lt;/p&gt;&lt;p&gt;Na cesti Lucija - Strunjan.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Nesreče Regionalna cesta slovenske Konjice - Tepanje je zaprta Dobrnežu. Zastoji Na cesti Bled - Lesce na Bledu. Na cesti Lucija - Strunjan. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F94" t="inlineStr"/>
@@ -5339,7 +5339,7 @@
       <c r="N94" t="inlineStr"/>
       <c r="O94" t="inlineStr">
         <is>
-          <t>Na cesti  Bled - Lesce na Bledu. Na cesti Lucija - Strunjan.</t>
+          <t>Na cesti Bled - Lesce na Bledu. Na cesti Lucija - Strunjan.</t>
         </is>
       </c>
       <c r="P94" t="inlineStr"/>
@@ -5382,7 +5382,7 @@
       <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Nesreče&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Slovenske Konjice - Tepanje je zaprta Dobrnežu. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Zastoji&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na cesti  Bled - Lesce na Bledu. &lt;/p&gt;&lt;p&gt;Na cesti Lucija - Strunjan.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Nesreče Regionalna cesta Slovenske Konjice - Tepanje je zaprta Dobrnežu. Zastoji Na cesti Bled - Lesce na Bledu. Na cesti Lucija - Strunjan. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F95" t="inlineStr"/>
@@ -5400,7 +5400,7 @@
       <c r="N95" t="inlineStr"/>
       <c r="O95" t="inlineStr">
         <is>
-          <t>Na cesti  Bled - Lesce na Bledu. Na cesti Lucija - Strunjan.</t>
+          <t>Na cesti Bled - Lesce na Bledu. Na cesti Lucija - Strunjan.</t>
         </is>
       </c>
       <c r="P95" t="inlineStr"/>
@@ -5437,13 +5437,13 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t xml:space="preserve">DARS Urh Šelih, PIC </t>
+          <t>DARS Urh Šelih, PIC</t>
         </is>
       </c>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Zastoji&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Na cesti  Bled - Lesce na Bledu. &lt;/p&gt;&lt;p&gt;Na cesti Lucija - Strunjan.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Zastoji Na cesti Bled - Lesce na Bledu. Na cesti Lucija - Strunjan. Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F96" t="inlineStr"/>
@@ -5457,7 +5457,7 @@
       <c r="N96" t="inlineStr"/>
       <c r="O96" t="inlineStr">
         <is>
-          <t>Na cesti  Bled - Lesce na Bledu. Na cesti Lucija - Strunjan.</t>
+          <t>Na cesti Bled - Lesce na Bledu. Na cesti Lucija - Strunjan.</t>
         </is>
       </c>
       <c r="P96" t="inlineStr"/>
@@ -5494,13 +5494,13 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t xml:space="preserve">DARS Urh Šelih, PIC </t>
+          <t>DARS Urh Šelih, PIC</t>
         </is>
       </c>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Opozorila&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Opozorila Danes do 22. ure velja splošna prepoved prometa za tovorna vozila nad 7,5 tone. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F97" t="inlineStr"/>
@@ -5547,13 +5547,13 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DARS Janko Poženel, GNC</t>
+          <t>DARS Janko Poženel, GNC</t>
         </is>
       </c>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F98" t="inlineStr"/>
@@ -5596,13 +5596,13 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DARS Janko Poženel, GNC</t>
+          <t>DARS Janko Poženel, GNC</t>
         </is>
       </c>
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F99" t="inlineStr"/>
@@ -5645,13 +5645,13 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DARS Janko Poženel, GNC</t>
+          <t>DARS Janko Poženel, GNC</t>
         </is>
       </c>
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F100" t="inlineStr"/>
@@ -5694,13 +5694,13 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DARS Janko Poženel, GNC</t>
+          <t>DARS Janko Poženel, GNC</t>
         </is>
       </c>
       <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr">
         <is>
-          <t>&lt;p&gt;&lt;strong&gt;Mejni prehodi&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Čakalna doba je na mejnem prehodu Gruškovje.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Dela&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.&lt;/p&gt;</t>
+          <t>Mejni prehodi Čakalna doba je na mejnem prehodu Gruškovje. Dela Regionalna cesta Javornik - Gorje bo zaradi rekonstrukcije ceste skozi naselje Gorje zaprta do 30. aprila. Obvoz je urejen na relaciji Bled - Lesce - Žirovnica - Javornik - Lipce in obratno.</t>
         </is>
       </c>
       <c r="F101" t="inlineStr"/>

</xml_diff>